<commit_message>
changes to inverts biomass pools N
</commit_message>
<xml_diff>
--- a/R/Scaling_biomass_logfile_output.xlsx
+++ b/R/Scaling_biomass_logfile_output.xlsx
@@ -717,7 +717,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -728,6 +728,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -743,11 +749,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14024,8 +14031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DA93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14038,7 +14045,9 @@
     <col min="6" max="6" width="5.42578125"/>
     <col min="7" max="7" width="8.5703125"/>
     <col min="8" max="8" width="2.7109375"/>
-    <col min="9" max="17" width="11.5703125"/>
+    <col min="9" max="13" width="11.5703125"/>
+    <col min="14" max="14" width="11.5703125" style="4"/>
+    <col min="15" max="17" width="11.5703125"/>
     <col min="18" max="18" width="8.5703125"/>
     <col min="19" max="1025" width="11.5703125"/>
   </cols>
@@ -14051,7 +14060,7 @@
       <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>98</v>
       </c>
       <c r="P1" t="s">
@@ -14108,7 +14117,7 @@
         <f t="shared" ref="L3:L34" si="0">I3/K3</f>
         <v>32334.653034096471</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="4">
         <v>6637.5</v>
       </c>
       <c r="P3">
@@ -14157,7 +14166,7 @@
         <f t="shared" si="0"/>
         <v>2822.7333005944411</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>4510.6719999999996</v>
       </c>
       <c r="P4">
@@ -14206,7 +14215,7 @@
         <f t="shared" si="0"/>
         <v>26200.03927260658</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="4">
         <v>80218.806890000007</v>
       </c>
       <c r="P5">
@@ -14255,7 +14264,7 @@
         <f t="shared" si="0"/>
         <v>5995.7992292521321</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>2697</v>
       </c>
       <c r="P6">
@@ -14304,7 +14313,7 @@
         <f t="shared" si="0"/>
         <v>111670.90064445119</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="4">
         <v>12347.108630000001</v>
       </c>
       <c r="P7">
@@ -14353,7 +14362,7 @@
         <f t="shared" si="0"/>
         <v>1206810.5644298124</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="4">
         <v>3907.9740299999999</v>
       </c>
       <c r="P8">
@@ -14402,7 +14411,7 @@
         <f t="shared" si="0"/>
         <v>577507.28635779093</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="4">
         <v>35892.089209999998</v>
       </c>
       <c r="P9">
@@ -14451,7 +14460,7 @@
         <f t="shared" si="0"/>
         <v>139983.37891277645</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="4">
         <v>21423.01856</v>
       </c>
       <c r="P10">
@@ -14500,7 +14509,7 @@
         <f t="shared" si="0"/>
         <v>71135.970886628784</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="4">
         <v>8105.2905899999996</v>
       </c>
       <c r="P11">
@@ -14549,7 +14558,7 @@
         <f t="shared" si="0"/>
         <v>14894885.539508017</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="4">
         <v>3646.2221399999999</v>
       </c>
       <c r="P12">
@@ -14598,7 +14607,7 @@
         <f t="shared" si="0"/>
         <v>225341.40876559602</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="4">
         <v>38854.992890000001</v>
       </c>
       <c r="P13">
@@ -14647,7 +14656,7 @@
         <f t="shared" si="0"/>
         <v>5957.3232948961004</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="4">
         <v>98.229510000000005</v>
       </c>
       <c r="P14">
@@ -14696,7 +14705,7 @@
         <f t="shared" si="0"/>
         <v>15827.914287452229</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="4">
         <v>1596.4079999999999</v>
       </c>
       <c r="P15">
@@ -14745,7 +14754,7 @@
         <f t="shared" si="0"/>
         <v>1648.0158820501817</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="4">
         <v>2273.672</v>
       </c>
       <c r="P16">
@@ -14794,7 +14803,7 @@
         <f t="shared" si="0"/>
         <v>16528.972870475995</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="4">
         <v>967.52</v>
       </c>
       <c r="P17">
@@ -14843,7 +14852,7 @@
         <f t="shared" si="0"/>
         <v>49.602847100924279</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="4">
         <v>4.8584350000000001</v>
       </c>
       <c r="P18">
@@ -14892,7 +14901,7 @@
         <f t="shared" si="0"/>
         <v>147735.16644666647</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="4">
         <v>5673.2709999999997</v>
       </c>
       <c r="P19">
@@ -14941,7 +14950,7 @@
         <f t="shared" si="0"/>
         <v>222997.36239896627</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="4">
         <v>12508.14644</v>
       </c>
       <c r="P20">
@@ -14990,7 +14999,7 @@
         <f t="shared" si="0"/>
         <v>10612.170183549215</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="4">
         <v>2343.3339999999998</v>
       </c>
       <c r="P21">
@@ -15039,7 +15048,7 @@
         <f t="shared" si="0"/>
         <v>10288.676864916613</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="4">
         <v>66381.201029999997</v>
       </c>
       <c r="P22">
@@ -15088,7 +15097,7 @@
         <f t="shared" si="0"/>
         <v>2694.3908743179663</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="4">
         <v>3164.95</v>
       </c>
       <c r="P23">
@@ -15137,7 +15146,7 @@
         <f t="shared" si="0"/>
         <v>31106.573378771598</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="4">
         <v>4742.7510000000002</v>
       </c>
       <c r="P24">
@@ -15186,7 +15195,7 @@
         <f t="shared" si="0"/>
         <v>403854.12366757158</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="4">
         <v>312490.47648000001</v>
       </c>
       <c r="P25">
@@ -15235,7 +15244,7 @@
         <f t="shared" si="0"/>
         <v>96441.722771503657</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="4">
         <v>124595.38234</v>
       </c>
       <c r="P26">
@@ -15284,7 +15293,7 @@
         <f t="shared" si="0"/>
         <v>509609.91366317705</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="4">
         <v>639.21481000000006</v>
       </c>
       <c r="P27">
@@ -15333,7 +15342,7 @@
         <f t="shared" si="0"/>
         <v>8018910.9210629696</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="4">
         <v>247495.45460999999</v>
       </c>
       <c r="P28">
@@ -15382,7 +15391,7 @@
         <f t="shared" si="0"/>
         <v>1422359.9165243958</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="4">
         <v>68851.370939999993</v>
       </c>
       <c r="P29">
@@ -15431,7 +15440,7 @@
         <f t="shared" si="0"/>
         <v>1703501.7570472998</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="4">
         <v>858.70898</v>
       </c>
       <c r="P30">
@@ -15480,7 +15489,7 @@
         <f t="shared" si="0"/>
         <v>729671.67014333291</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="4">
         <v>8099.2672199999997</v>
       </c>
       <c r="P31">
@@ -15529,7 +15538,7 @@
         <f t="shared" si="0"/>
         <v>6475507.3071110779</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="4">
         <v>466.91953999999998</v>
       </c>
       <c r="P32">
@@ -15578,7 +15587,7 @@
         <f t="shared" si="0"/>
         <v>144879.66255601178</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="4">
         <v>204570.50472</v>
       </c>
       <c r="P33">
@@ -15627,7 +15636,7 @@
         <f t="shared" si="0"/>
         <v>1825653.1900334202</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="4">
         <v>68242.971520000006</v>
       </c>
       <c r="P34">
@@ -15676,7 +15685,7 @@
         <f t="shared" ref="L35:L66" si="2">I35/K35</f>
         <v>13241005.419341654</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="4">
         <v>26.160060000000001</v>
       </c>
       <c r="P35">
@@ -15725,7 +15734,7 @@
         <f t="shared" si="2"/>
         <v>1439847.8832143997</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="4">
         <v>444.32128</v>
       </c>
       <c r="P36">
@@ -15774,7 +15783,7 @@
         <f t="shared" si="2"/>
         <v>4667431.6609816672</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="4">
         <v>2041.1949999999999</v>
       </c>
       <c r="P37">
@@ -15823,7 +15832,7 @@
         <f t="shared" si="2"/>
         <v>1378593.9375233175</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="4">
         <v>385.52397999999999</v>
       </c>
       <c r="P38">
@@ -15872,7 +15881,7 @@
         <f t="shared" si="2"/>
         <v>1576378.5021292702</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="4">
         <v>6193.6677499999996</v>
       </c>
       <c r="P39">
@@ -15921,7 +15930,7 @@
         <f t="shared" si="2"/>
         <v>12307508.263326706</v>
       </c>
-      <c r="N40">
+      <c r="N40" s="4">
         <v>638.52646000000004</v>
       </c>
       <c r="P40">
@@ -15970,7 +15979,7 @@
         <f t="shared" si="2"/>
         <v>411424.26558740315</v>
       </c>
-      <c r="N41">
+      <c r="N41" s="4">
         <v>287990.48550000001</v>
       </c>
       <c r="P41">
@@ -16019,7 +16028,7 @@
         <f t="shared" si="2"/>
         <v>457742.32358836627</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="4">
         <v>837622.32530000003</v>
       </c>
       <c r="P42">
@@ -16068,7 +16077,7 @@
         <f t="shared" si="2"/>
         <v>24584.945959613968</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="4">
         <v>88958.136549999996</v>
       </c>
       <c r="P43">
@@ -16117,7 +16126,7 @@
         <f t="shared" si="2"/>
         <v>3958043.864978971</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="4">
         <v>633208.32400000002</v>
       </c>
       <c r="P44">
@@ -16166,7 +16175,7 @@
         <f t="shared" si="2"/>
         <v>44682.626845092025</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="4">
         <v>17226.46154</v>
       </c>
       <c r="P45">
@@ -16215,7 +16224,7 @@
         <f t="shared" si="2"/>
         <v>191776.89952824815</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="4">
         <v>3484.8640300000002</v>
       </c>
       <c r="P46">
@@ -16264,7 +16273,7 @@
         <f t="shared" si="2"/>
         <v>2433692.147976046</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="4">
         <v>1253.7247</v>
       </c>
       <c r="P47">
@@ -16313,7 +16322,7 @@
         <f t="shared" si="2"/>
         <v>3949.3787702076143</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="4">
         <v>2873.4</v>
       </c>
       <c r="P48">
@@ -16362,7 +16371,7 @@
         <f t="shared" si="2"/>
         <v>6187.1282814849856</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="4">
         <v>1436.7</v>
       </c>
       <c r="P49">
@@ -16411,7 +16420,7 @@
         <f t="shared" si="2"/>
         <v>18480.448327821337</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="4">
         <v>3114.6878999999999</v>
       </c>
       <c r="P50">
@@ -16460,7 +16469,7 @@
         <f t="shared" si="2"/>
         <v>2716651.003264348</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="4">
         <v>128678.71575</v>
       </c>
       <c r="P51">
@@ -16509,7 +16518,7 @@
         <f t="shared" si="2"/>
         <v>541928.45997168473</v>
       </c>
-      <c r="N52">
+      <c r="N52" s="4">
         <v>130790.82432</v>
       </c>
       <c r="P52">
@@ -16558,7 +16567,7 @@
         <f t="shared" si="2"/>
         <v>3629917.3480213298</v>
       </c>
-      <c r="N53">
+      <c r="N53" s="4">
         <v>181995.72683</v>
       </c>
       <c r="P53">
@@ -16607,7 +16616,7 @@
         <f t="shared" si="2"/>
         <v>832.33159773690284</v>
       </c>
-      <c r="N54">
+      <c r="N54" s="4">
         <v>1808.5</v>
       </c>
       <c r="P54">
@@ -16656,7 +16665,7 @@
         <f t="shared" si="2"/>
         <v>17644.875052242092</v>
       </c>
-      <c r="N55">
+      <c r="N55" s="4">
         <v>7660.8</v>
       </c>
       <c r="P55">
@@ -16705,7 +16714,7 @@
         <f t="shared" si="2"/>
         <v>2298.431124876035</v>
       </c>
-      <c r="N56">
+      <c r="N56" s="4">
         <v>803.2</v>
       </c>
       <c r="P56">
@@ -16754,7 +16763,7 @@
         <f t="shared" si="2"/>
         <v>100092.98783058119</v>
       </c>
-      <c r="N57">
+      <c r="N57" s="4">
         <v>18046.14</v>
       </c>
       <c r="P57">
@@ -16803,7 +16812,7 @@
         <f t="shared" si="2"/>
         <v>81860.843754175454</v>
       </c>
-      <c r="N58">
+      <c r="N58" s="4">
         <v>72184.56</v>
       </c>
       <c r="P58">
@@ -16852,7 +16861,7 @@
         <f t="shared" si="2"/>
         <v>10617.124344696853</v>
       </c>
-      <c r="N59">
+      <c r="N59" s="4">
         <v>11998.44</v>
       </c>
       <c r="P59">
@@ -16901,7 +16910,7 @@
         <f t="shared" si="2"/>
         <v>631039.9356368247</v>
       </c>
-      <c r="N60">
+      <c r="N60" s="4">
         <v>7998.96</v>
       </c>
       <c r="P60">
@@ -16950,7 +16959,7 @@
         <f t="shared" si="2"/>
         <v>1251262.3298339883</v>
       </c>
-      <c r="N61">
+      <c r="N61" s="4">
         <v>2616.0059999999999</v>
       </c>
       <c r="P61">
@@ -16999,7 +17008,7 @@
         <f t="shared" si="2"/>
         <v>89206.458132</v>
       </c>
-      <c r="N62">
+      <c r="N62" s="4">
         <v>44619.42</v>
       </c>
       <c r="P62" s="3">
@@ -17048,7 +17057,7 @@
         <f t="shared" si="2"/>
         <v>59470.972088000002</v>
       </c>
-      <c r="N63">
+      <c r="N63" s="4">
         <v>29746.28</v>
       </c>
       <c r="P63" s="3">
@@ -17097,7 +17106,7 @@
         <f t="shared" si="2"/>
         <v>56361.683889</v>
       </c>
-      <c r="N64">
+      <c r="N64" s="4">
         <v>4656.1183199999996</v>
       </c>
       <c r="P64" s="3">
@@ -17146,7 +17155,7 @@
         <f t="shared" si="2"/>
         <v>18111.507552999999</v>
       </c>
-      <c r="N65">
+      <c r="N65" s="4">
         <v>6.5920009999999998</v>
       </c>
       <c r="P65" s="3">
@@ -17195,7 +17204,7 @@
         <f t="shared" si="2"/>
         <v>18111.507552999999</v>
       </c>
-      <c r="N66">
+      <c r="N66" s="4">
         <v>181253.05</v>
       </c>
       <c r="P66" s="3">
@@ -17241,10 +17250,10 @@
         <v>1</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L98" si="4">I67/K67</f>
+        <f t="shared" ref="L67:L91" si="4">I67/K67</f>
         <v>18017.283443</v>
       </c>
-      <c r="N67">
+      <c r="N67" s="4">
         <v>1540650.925</v>
       </c>
       <c r="P67" s="3">
@@ -17293,7 +17302,7 @@
         <f t="shared" si="4"/>
         <v>50305.658228</v>
       </c>
-      <c r="N68">
+      <c r="N68" s="4">
         <v>5035438.5999999996</v>
       </c>
       <c r="P68" s="3">
@@ -17342,7 +17351,7 @@
         <f t="shared" si="4"/>
         <v>20548.220792</v>
       </c>
-      <c r="N69">
+      <c r="N69" s="4">
         <v>20570</v>
       </c>
       <c r="P69" s="3">
@@ -17391,7 +17400,7 @@
         <f t="shared" si="4"/>
         <v>8411.5164480000003</v>
       </c>
-      <c r="N70">
+      <c r="N70" s="4">
         <v>7.1902939999999997</v>
       </c>
       <c r="P70" s="3">
@@ -17440,7 +17449,7 @@
         <f t="shared" si="4"/>
         <v>803070.14760000003</v>
       </c>
-      <c r="N71">
+      <c r="N71" s="4">
         <v>723132.18</v>
       </c>
       <c r="P71" s="3">
@@ -17489,7 +17498,7 @@
         <f t="shared" si="4"/>
         <v>38931.483149</v>
       </c>
-      <c r="N72">
+      <c r="N72" s="4">
         <v>1704.171</v>
       </c>
       <c r="P72" s="3">
@@ -17538,7 +17547,7 @@
         <f t="shared" si="4"/>
         <v>38931.483149</v>
       </c>
-      <c r="N73">
+      <c r="N73" s="4">
         <v>3018.587</v>
       </c>
       <c r="P73" s="3">
@@ -17587,7 +17596,7 @@
         <f t="shared" si="4"/>
         <v>1014574.10599</v>
       </c>
-      <c r="N74">
+      <c r="N74" s="4">
         <v>88497.144625719302</v>
       </c>
       <c r="P74" s="3">
@@ -17636,7 +17645,7 @@
         <f t="shared" si="4"/>
         <v>37503.620778999997</v>
       </c>
-      <c r="N75">
+      <c r="N75" s="4">
         <v>375230138.30000001</v>
       </c>
       <c r="P75" s="3">
@@ -17685,7 +17694,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N76" t="e">
+      <c r="N76" s="4" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
@@ -17732,7 +17741,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N77" t="e">
+      <c r="N77" s="4" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
@@ -17779,7 +17788,7 @@
         <f t="shared" si="4"/>
         <v>602095.65274299996</v>
       </c>
-      <c r="N78">
+      <c r="N78" s="4">
         <v>6025037.2999999998</v>
       </c>
       <c r="P78" s="3">
@@ -17828,7 +17837,7 @@
         <f t="shared" si="4"/>
         <v>1737186.756822</v>
       </c>
-      <c r="N79">
+      <c r="N79" s="4">
         <v>151644.371947782</v>
       </c>
       <c r="P79" s="3">
@@ -17877,7 +17886,7 @@
         <f t="shared" si="4"/>
         <v>205524.48199500001</v>
       </c>
-      <c r="N80">
+      <c r="N80" s="4">
         <v>548371.06777746405</v>
       </c>
       <c r="P80" s="3">
@@ -17926,7 +17935,7 @@
         <f t="shared" si="4"/>
         <v>68444.349277999994</v>
       </c>
-      <c r="N81">
+      <c r="N81" s="4">
         <v>201134.73789574299</v>
       </c>
       <c r="P81" s="3">
@@ -17975,7 +17984,7 @@
         <f t="shared" si="4"/>
         <v>68444.349277999994</v>
       </c>
-      <c r="N82">
+      <c r="N82" s="4">
         <v>163315.90861250801</v>
       </c>
       <c r="P82" s="3">
@@ -18024,7 +18033,7 @@
         <f t="shared" si="4"/>
         <v>1087701.814337</v>
       </c>
-      <c r="N83">
+      <c r="N83" s="4">
         <v>94440.610721329402</v>
       </c>
       <c r="P83" s="3">
@@ -18073,7 +18082,7 @@
         <f t="shared" si="4"/>
         <v>4285665.1151689999</v>
       </c>
-      <c r="N84">
+      <c r="N84" s="4">
         <v>374087.87270517001</v>
       </c>
       <c r="P84" s="3">
@@ -18122,7 +18131,7 @@
         <f t="shared" si="4"/>
         <v>31811.945437999999</v>
       </c>
-      <c r="N85">
+      <c r="N85" s="4">
         <v>31842.799999999999</v>
       </c>
       <c r="P85" s="3">
@@ -18171,7 +18180,7 @@
         <f t="shared" si="4"/>
         <v>15052.391319</v>
       </c>
-      <c r="N86">
+      <c r="N86" s="4">
         <v>15062593.300000001</v>
       </c>
       <c r="P86" s="3">
@@ -18220,7 +18229,7 @@
         <f t="shared" si="4"/>
         <v>6020.9565270000003</v>
       </c>
-      <c r="N87">
+      <c r="N87" s="4">
         <v>60250373.299999997</v>
       </c>
       <c r="P87" s="3">
@@ -18269,7 +18278,7 @@
         <f t="shared" si="4"/>
         <v>15052391.318573</v>
       </c>
-      <c r="N88" t="e">
+      <c r="N88" s="4" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
@@ -18316,7 +18325,7 @@
         <f t="shared" si="4"/>
         <v>60209.565274</v>
       </c>
-      <c r="N89" t="e">
+      <c r="N89" s="4" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
@@ -18363,7 +18372,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N90" t="e">
+      <c r="N90" s="4" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
@@ -18410,7 +18419,7 @@
         <f t="shared" si="4"/>
         <v>329357996.66267502</v>
       </c>
-      <c r="N91" t="e">
+      <c r="N91" s="4" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>

</xml_diff>

<commit_message>
fixed init file time steps from 2 to 1, error caused by previous commit
</commit_message>
<xml_diff>
--- a/R/Scaling_biomass_logfile_output.xlsx
+++ b/R/Scaling_biomass_logfile_output.xlsx
@@ -1402,7 +1402,7 @@
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H76" activeCellId="1" sqref="AI111:AI120 H76"/>
+      <selection pane="topLeft" activeCell="H76" activeCellId="0" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4010,7 +4010,7 @@
   <dimension ref="A1:AG116"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N64" activeCellId="1" sqref="AI111:AI120 N64"/>
+      <selection pane="topLeft" activeCell="N64" activeCellId="0" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8802,7 +8802,7 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C78" activeCellId="1" sqref="AI111:AI120 C78"/>
+      <selection pane="topLeft" activeCell="C78" activeCellId="0" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10365,7 +10365,7 @@
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AI111:AI120 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12973,7 +12973,7 @@
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AI111:AI120 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15581,7 +15581,7 @@
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L31" activeCellId="1" sqref="AI111:AI120 L31"/>
+      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18189,7 +18189,7 @@
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H76" activeCellId="1" sqref="AI111:AI120 H76"/>
+      <selection pane="topLeft" activeCell="H76" activeCellId="0" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20797,7 +20797,7 @@
   <dimension ref="A1:DA93"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N87" activeCellId="1" sqref="AI111:AI120 N87"/>
+      <selection pane="topLeft" activeCell="N87" activeCellId="0" sqref="N87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25485,7 +25485,7 @@
   <dimension ref="A1:AS93"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P64" activeCellId="1" sqref="AI111:AI120 P64"/>
+      <selection pane="topLeft" activeCell="P64" activeCellId="0" sqref="P64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29631,7 +29631,7 @@
   <dimension ref="A1:V93"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="AI111:AI120 E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32701,10 +32701,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI122"/>
+  <dimension ref="A1:AJ124"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI111" activeCellId="0" sqref="AI111:AI120"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE124" activeCellId="0" sqref="AE124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36912,16 +36912,19 @@
         <v>0.0077464794</v>
       </c>
       <c r="AE111" s="0" t="n">
-        <v>0.0482734857</v>
+        <v>0.0311133611999999</v>
       </c>
       <c r="AG111" s="0" t="n">
         <f aca="false">SUM(B111:AE111)</f>
-        <v>1.0171601245</v>
+        <v>1</v>
       </c>
       <c r="AI111" s="0" t="n">
         <f aca="false">AE111-AG111+1</f>
         <v>0.0311133612000001</v>
       </c>
+      <c r="AJ111" s="0" t="n">
+        <v>0.0311133611999999</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AG112" s="0" t="n">
@@ -37038,11 +37041,11 @@
         <v>0.0077464794</v>
       </c>
       <c r="AE114" s="0" t="n">
-        <v>0.0482734857</v>
+        <v>0.0311133611999999</v>
       </c>
       <c r="AG114" s="0" t="n">
         <f aca="false">SUM(B114:AE114)</f>
-        <v>1.0171601245</v>
+        <v>1</v>
       </c>
       <c r="AI114" s="0" t="n">
         <f aca="false">AE114-AG114+1</f>
@@ -37164,16 +37167,19 @@
         <v>0.038657821</v>
       </c>
       <c r="AE117" s="0" t="n">
-        <v>0.0428777881</v>
+        <v>0.0120835238999999</v>
       </c>
       <c r="AG117" s="0" t="n">
         <f aca="false">SUM(B117:AE117)</f>
-        <v>1.0307942642</v>
+        <v>1</v>
       </c>
       <c r="AI117" s="0" t="n">
         <f aca="false">AE117-AG117+1</f>
         <v>0.0120835238999999</v>
       </c>
+      <c r="AJ117" s="0" t="n">
+        <v>0.0120835238999999</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AG118" s="0" t="n">
@@ -37290,11 +37296,11 @@
         <v>0.038657821</v>
       </c>
       <c r="AE120" s="0" t="n">
-        <v>0.0428777881</v>
+        <v>0.0120835238999999</v>
       </c>
       <c r="AG120" s="0" t="n">
         <f aca="false">SUM(B120:AE120)</f>
-        <v>1.0307942642</v>
+        <v>1</v>
       </c>
       <c r="AI120" s="0" t="n">
         <f aca="false">AE120-AG120+1</f>
@@ -37304,7 +37310,103 @@
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="str">
         <f aca="false">"  "&amp;B120&amp;", "&amp;C120&amp;", "&amp;D120&amp;", "&amp;E120&amp;", "&amp;F120&amp;", "&amp;G120&amp;", "&amp;H120&amp;", "&amp;I120&amp;", "&amp;J120&amp;", "&amp;K120&amp;", "&amp;L120&amp;", "&amp;M120&amp;", "&amp;N120&amp;", "&amp;O120&amp;", "&amp;P120&amp;", "&amp;Q120&amp;", "&amp;R120&amp;", "&amp;S120&amp;", "&amp;T120&amp;", "&amp;U120&amp;", "&amp;V120&amp;", "&amp;W120&amp;", "&amp;X120&amp;", "&amp;Y120&amp;", "&amp;Z120&amp;", "&amp;AA120&amp;", "&amp;AB120&amp;", "&amp;AC120&amp;", "&amp;AD120&amp;", "&amp;AE120&amp;", "&amp;S120&amp;" ;"</f>
-        <v>  0.0373255751, 0.0419043562, 0.0368473015, 0.0228798557, 0.0307420495, 0.0428273817, 0.0366235091, 0.0295364766, 0.0237373898, 0.0336811514, 0.0352079621, 0.0210095621, 0.043341989, 0.0213170406, 0.0211525724, 0.0237544351, 0.0438039434, 0.0307942645, 0.0307942645, 0.0245440207, 0.0226432032, 0.0340607095, 0.0402417821, 0.0440278901, 0.0431754419, 0.044547291, 0.0450825727, 0.0436546636, 0.038657821, 0.0428777881, 0.0307942645 ;</v>
+        <v>  0.0373255751, 0.0419043562, 0.0368473015, 0.0228798557, 0.0307420495, 0.0428273817, 0.0366235091, 0.0295364766, 0.0237373898, 0.0336811514, 0.0352079621, 0.0210095621, 0.043341989, 0.0213170406, 0.0211525724, 0.0237544351, 0.0438039434, 0.0307942645, 0.0307942645, 0.0245440207, 0.0226432032, 0.0340607095, 0.0402417821, 0.0440278901, 0.0431754419, 0.044547291, 0.0450825727, 0.0436546636, 0.038657821, 0.0120835238999999, 0.0307942645 ;</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="D124" s="0" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="E124" s="0" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="F124" s="0" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="G124" s="0" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="H124" s="0" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="I124" s="0" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="J124" s="0" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="K124" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L124" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M124" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N124" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O124" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="P124" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="Q124" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="R124" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="S124" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="T124" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="U124" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="V124" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="W124" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="X124" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="Y124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG124" s="0" t="n">
+        <f aca="false">SUM(B124:AE124)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
on track to revise init numbers spatial dist
</commit_message>
<xml_diff>
--- a/R/Scaling_biomass_logfile_output.xlsx
+++ b/R/Scaling_biomass_logfile_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="820" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="820" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="20180619b" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="ISQ" sheetId="10" r:id="rId11"/>
     <sheet name="desiredBiomass" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -8996,7 +8996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG116"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N64" sqref="N64:N93"/>
     </sheetView>
   </sheetViews>
@@ -13780,8 +13780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28951,7 +28951,7 @@
         <v>1</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L98" si="4">I67/K67</f>
+        <f t="shared" ref="L67:L91" si="4">I67/K67</f>
         <v>18017.283443</v>
       </c>
       <c r="N67" s="1">
@@ -30415,7 +30415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
@@ -35197,7 +35197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS93"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
@@ -39335,7 +39335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C46" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
@@ -40660,7 +40660,7 @@
         <v>216250500000</v>
       </c>
       <c r="P34" s="2">
-        <f t="shared" ref="P33:P55" si="4">$P$31/20/5.7*B34/2/N34</f>
+        <f t="shared" ref="P34:P55" si="4">$P$31/20/5.7*B34/2/N34</f>
         <v>0.12704564479863081</v>
       </c>
     </row>

</xml_diff>

<commit_message>
progress toward updated biomass distribution for init
</commit_message>
<xml_diff>
--- a/R/Scaling_biomass_logfile_output.xlsx
+++ b/R/Scaling_biomass_logfile_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="820" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="820" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="20180619b" sheetId="1" r:id="rId1"/>
@@ -30415,8 +30415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35197,8 +35197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>